<commit_message>
Added a additional goal to sprint 2
</commit_message>
<xml_diff>
--- a/scrum/backlog.xlsx
+++ b/scrum/backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Backlog</t>
   </si>
@@ -75,7 +75,10 @@
     <t>Urs / Arun</t>
   </si>
   <si>
-    <t>Oli/Urs</t>
+    <t>Pictures</t>
+  </si>
+  <si>
+    <t>Urs/Arun</t>
   </si>
 </sst>
 </file>
@@ -385,7 +388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +500,7 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -519,7 +522,18 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>